<commit_message>
push finescale fishery composition supplementary table
</commit_message>
<xml_diff>
--- a/termREN/2023/supplementary/R_OUT - Recreational fishery fine-scale stock composition (Terminal Renfrew areas) 2023-output_from_04.xlsx
+++ b/termREN/2023/supplementary/R_OUT - Recreational fishery fine-scale stock composition (Terminal Renfrew areas) 2023-output_from_04.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -925,12 +925,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -970,12 +970,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1015,12 +1015,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1960,12 +1960,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2005,12 +2005,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2320,12 +2320,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Hatchery Not Found - Puget Sound South</t>
+          <t>Hatchery Unknown (DNA did not resolve)</t>
         </is>
       </c>
       <c r="G51">
@@ -2680,17 +2680,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Hatchery Puget Sound</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Robertson Creek</t>
         </is>
       </c>
       <c r="G52">
@@ -2700,10 +2700,10 @@
         <v>1</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -2725,17 +2725,17 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Puget Sound</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Not Found - Puget Sound South</t>
         </is>
       </c>
       <c r="G53">
@@ -2745,10 +2745,10 @@
         <v>1</v>
       </c>
       <c r="I53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -3400,30 +3400,30 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Nitinat River</t>
         </is>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I68">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -3445,17 +3445,17 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Robertson Creek</t>
         </is>
       </c>
       <c r="G69">
@@ -3465,7 +3465,7 @@
         <v>10</v>
       </c>
       <c r="I69">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J69">
         <v>4</v>
@@ -3490,30 +3490,30 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Thornton Creek (WCVI)</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Thornton Creek</t>
         </is>
       </c>
       <c r="G70">
         <v>0</v>
       </c>
       <c r="H70">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I70">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="J70">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K70">
         <v>0</v>
@@ -3535,30 +3535,30 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Unknown (DNA did not resolve)</t>
         </is>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I71">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -3580,27 +3580,27 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Hatchery Thornton Creek</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Hatchery Thornton Creek</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="G72">
         <v>0</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I72">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -3625,17 +3625,17 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="G73">
@@ -3645,10 +3645,10 @@
         <v>1</v>
       </c>
       <c r="I73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73">
         <v>0</v>
@@ -4165,17 +4165,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Thornton Creek (WCVI)</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Thornton Creek</t>
         </is>
       </c>
       <c r="G85">
@@ -4185,7 +4185,7 @@
         <v>1</v>
       </c>
       <c r="I85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J85">
         <v>0</v>
@@ -4210,17 +4210,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Hatchery Thornton Creek</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Hatchery Thornton Creek</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="G86">
@@ -4230,7 +4230,7 @@
         <v>1</v>
       </c>
       <c r="I86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J86">
         <v>0</v>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -4660,7 +4660,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -4705,7 +4705,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -4885,12 +4885,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -4930,12 +4930,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -5290,12 +5290,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -5335,12 +5335,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -5380,12 +5380,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -5515,12 +5515,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -5605,12 +5605,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -5650,12 +5650,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -6145,12 +6145,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -6190,12 +6190,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -6325,12 +6325,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -6370,12 +6370,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -6685,12 +6685,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -6730,12 +6730,12 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -6775,12 +6775,12 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -6910,12 +6910,12 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -7135,12 +7135,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -7180,12 +7180,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -7225,12 +7225,12 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -7585,12 +7585,12 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Hatchery Burman River</t>
+          <t>Hatchery Burman River (WCVI)</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -7630,12 +7630,12 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -7675,12 +7675,12 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -7855,7 +7855,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -7900,12 +7900,12 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Unknown Robertson Creek</t>
+          <t>Unknown Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -8530,12 +8530,12 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Natural Robertson Creek</t>
+          <t>Natural Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -8665,12 +8665,12 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -8710,12 +8710,12 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -8755,12 +8755,12 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -8890,12 +8890,12 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -9025,12 +9025,12 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -9070,12 +9070,12 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -9385,12 +9385,12 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -9430,12 +9430,12 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -9520,12 +9520,12 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>Natural Nitinat River</t>
+          <t>Natural Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -9565,12 +9565,12 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Natural Unknown (DNA did not resolve)</t>
+          <t>Natural Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -9700,12 +9700,12 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Unknown Nitinat River</t>
+          <t>Unknown Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -9970,7 +9970,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -10015,12 +10015,12 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -10060,12 +10060,12 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -10285,12 +10285,12 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -10330,12 +10330,12 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -10375,12 +10375,12 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -10555,12 +10555,12 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Natural Robertson Creek</t>
+          <t>Natural Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -10600,12 +10600,12 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -10645,12 +10645,12 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Natural Unknown (DNA did not resolve)</t>
+          <t>Natural Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -10780,12 +10780,12 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -10825,12 +10825,12 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -10870,12 +10870,12 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -11230,12 +11230,12 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -11275,12 +11275,12 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -11645,7 +11645,7 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>Hatchery Not Found - Puget Sound North</t>
+          <t>Hatchery Skagit River</t>
         </is>
       </c>
       <c r="G251">
@@ -11690,17 +11690,17 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>Hatchery Skagit River</t>
+          <t>Hatchery Soos Creek Hatchery</t>
         </is>
       </c>
       <c r="G252">
         <v>0</v>
       </c>
       <c r="H252">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I252">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J252">
         <v>0</v>
@@ -11735,17 +11735,17 @@
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>Hatchery Soos Creek Hatchery</t>
+          <t>Hatchery Unknown (DNA did not resolve)</t>
         </is>
       </c>
       <c r="G253">
         <v>0</v>
       </c>
       <c r="H253">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J253">
         <v>0</v>
@@ -11770,27 +11770,27 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Hatchery Puget Sound</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Robertson Creek</t>
         </is>
       </c>
       <c r="G254">
         <v>0</v>
       </c>
       <c r="H254">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I254">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J254">
         <v>0</v>
@@ -11815,17 +11815,17 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Puget Sound</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Not Found - Puget Sound North</t>
         </is>
       </c>
       <c r="G255">
@@ -11835,7 +11835,7 @@
         <v>1</v>
       </c>
       <c r="I255">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J255">
         <v>0</v>
@@ -11860,27 +11860,27 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="G256">
         <v>0</v>
       </c>
       <c r="H256">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I256">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J256">
         <v>0</v>
@@ -11950,12 +11950,12 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -12040,12 +12040,12 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -12175,17 +12175,17 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Robertson Creek</t>
         </is>
       </c>
       <c r="G263">
@@ -12220,17 +12220,17 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="G264">
@@ -12265,12 +12265,12 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown San Juan River</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Unknown San Juan River</t>
+          <t>Unknown San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -12625,7 +12625,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -13030,12 +13030,12 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -13075,17 +13075,17 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Tranquil River (WCVI)</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Tranquil River</t>
         </is>
       </c>
       <c r="G283">
@@ -13098,7 +13098,7 @@
         <v>1</v>
       </c>
       <c r="J283">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -13120,17 +13120,17 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Hatchery Tranquil River</t>
+          <t>Hatchery Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>Hatchery Tranquil River</t>
+          <t>Hatchery Unknown (DNA did not resolve)</t>
         </is>
       </c>
       <c r="G284">
@@ -13143,7 +13143,7 @@
         <v>1</v>
       </c>
       <c r="J284">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K284">
         <v>0</v>
@@ -13165,17 +13165,17 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="G285">
@@ -13300,12 +13300,12 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -13525,12 +13525,12 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -13930,12 +13930,12 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -13975,12 +13975,12 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -14020,7 +14020,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -14290,12 +14290,12 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -14335,12 +14335,12 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -14470,12 +14470,12 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Hatchery Gold River</t>
+          <t>Hatchery Gold River (WCVI)</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -14515,12 +14515,12 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -15550,17 +15550,17 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>Hatchery Unknown</t>
+          <t>Hatchery Robertson Creek</t>
         </is>
       </c>
       <c r="G338">
@@ -15570,10 +15570,10 @@
         <v>0</v>
       </c>
       <c r="I338">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J338">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K338">
         <v>0</v>
@@ -15595,17 +15595,17 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Unknown (DNA did not resolve)</t>
         </is>
       </c>
       <c r="G339">
@@ -15615,10 +15615,10 @@
         <v>0</v>
       </c>
       <c r="I339">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J339">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K339">
         <v>0</v>
@@ -15640,17 +15640,17 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="G340">
@@ -15660,7 +15660,7 @@
         <v>0</v>
       </c>
       <c r="I340">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J340">
         <v>0</v>
@@ -16225,12 +16225,12 @@
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -16405,7 +16405,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E357" t="inlineStr">
@@ -16450,7 +16450,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E358" t="inlineStr">
@@ -16765,7 +16765,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E365" t="inlineStr">
@@ -16900,12 +16900,12 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -17395,12 +17395,12 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -17440,12 +17440,12 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Hatchery Thornton Creek</t>
+          <t>Hatchery Thornton Creek (WCVI)</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -17485,12 +17485,12 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Hatchery Unknown (DNA did not resolve)</t>
+          <t>Hatchery Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -17530,7 +17530,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E382" t="inlineStr">
@@ -17575,7 +17575,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E383" t="inlineStr">
@@ -17980,12 +17980,12 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>Hatchery Kennedy River</t>
+          <t>Hatchery Kennedy River (WCVI)</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -18025,12 +18025,12 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -18430,12 +18430,12 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -18790,12 +18790,12 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -18835,12 +18835,12 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>Hatchery Thornton Creek</t>
+          <t>Hatchery Thornton Creek (WCVI)</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -19195,12 +19195,12 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Natural Nitinat River</t>
+          <t>Natural Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -19240,12 +19240,12 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -19420,17 +19420,17 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E424" t="inlineStr">
         <is>
-          <t>Unknown Unknown</t>
+          <t>Unknown Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>Unknown Unknown</t>
+          <t>Unknown Nitinat River</t>
         </is>
       </c>
       <c r="G424">
@@ -19440,10 +19440,10 @@
         <v>0</v>
       </c>
       <c r="I424">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J424">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K424">
         <v>0</v>
@@ -19465,17 +19465,17 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E425" t="inlineStr">
         <is>
-          <t>Unknown Nitinat River</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>Unknown Nitinat River</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="G425">
@@ -19485,10 +19485,10 @@
         <v>0</v>
       </c>
       <c r="I425">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J425">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K425">
         <v>0</v>
@@ -19645,12 +19645,12 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E429" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -19915,17 +19915,17 @@
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>Natural Unknown</t>
+          <t>Natural San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Natural Unknown</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="G435">
@@ -19935,7 +19935,7 @@
         <v>0</v>
       </c>
       <c r="I435">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J435">
         <v>0</v>
@@ -19960,17 +19960,17 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="G436">
@@ -19980,7 +19980,7 @@
         <v>0</v>
       </c>
       <c r="I436">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J436">
         <v>0</v>
@@ -20185,12 +20185,12 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>Unknown Robertson Creek</t>
+          <t>Unknown Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -20230,12 +20230,12 @@
       </c>
       <c r="D442" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown San Juan River</t>
         </is>
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>Unknown San Juan River</t>
+          <t>Unknown San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -20320,12 +20320,12 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E444" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -20860,12 +20860,12 @@
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>Natural Nitinat River</t>
+          <t>Natural Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
@@ -21400,17 +21400,17 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Sarita River (WCVI)</t>
         </is>
       </c>
       <c r="F468" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery Sarita River</t>
         </is>
       </c>
       <c r="G468">
@@ -21445,17 +21445,17 @@
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E469" t="inlineStr">
         <is>
-          <t>Hatchery Sarita River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F469" t="inlineStr">
         <is>
-          <t>Hatchery Sarita River</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="G469">
@@ -21760,7 +21760,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E476" t="inlineStr">
@@ -22255,17 +22255,17 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E487" t="inlineStr">
         <is>
-          <t>Unknown Unknown</t>
+          <t>Unknown Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F487" t="inlineStr">
         <is>
-          <t>Unknown Unknown</t>
+          <t>Unknown Robertson Creek</t>
         </is>
       </c>
       <c r="G487">
@@ -22275,7 +22275,7 @@
         <v>0</v>
       </c>
       <c r="I487">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J487">
         <v>0</v>
@@ -22300,17 +22300,17 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown San Juan River</t>
         </is>
       </c>
       <c r="E488" t="inlineStr">
         <is>
-          <t>Unknown Robertson Creek</t>
+          <t>Unknown San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F488" t="inlineStr">
         <is>
-          <t>Unknown Robertson Creek</t>
+          <t>Unknown San Juan River</t>
         </is>
       </c>
       <c r="G488">
@@ -22320,10 +22320,10 @@
         <v>0</v>
       </c>
       <c r="I488">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J488">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K488">
         <v>0</v>
@@ -22345,17 +22345,17 @@
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E489" t="inlineStr">
         <is>
-          <t>Unknown San Juan River</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="F489" t="inlineStr">
         <is>
-          <t>Unknown San Juan River</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="G489">
@@ -22365,10 +22365,10 @@
         <v>0</v>
       </c>
       <c r="I489">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J489">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K489">
         <v>0</v>
@@ -22570,12 +22570,12 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E494" t="inlineStr">
         <is>
-          <t>Hatchery Marble River</t>
+          <t>Hatchery Marble River (WCVI)</t>
         </is>
       </c>
       <c r="F494" t="inlineStr">
@@ -22705,12 +22705,12 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E497" t="inlineStr">
         <is>
-          <t>Unknown Robertson Creek</t>
+          <t>Unknown Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F497" t="inlineStr">
@@ -22750,12 +22750,12 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E498" t="inlineStr">
         <is>
-          <t>Unknown Unknown (DNA did not resolve)</t>
+          <t>Unknown Unknown (DNA did not resolve) (WCVI)</t>
         </is>
       </c>
       <c r="F498" t="inlineStr">
@@ -22840,12 +22840,12 @@
       </c>
       <c r="D500" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E500" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F500" t="inlineStr">
@@ -22885,12 +22885,12 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E501" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F501" t="inlineStr">
@@ -23245,17 +23245,17 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E509" t="inlineStr">
         <is>
-          <t>Unknown Unknown</t>
+          <t>Unknown Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F509" t="inlineStr">
         <is>
-          <t>Unknown Unknown</t>
+          <t>Unknown Nitinat River</t>
         </is>
       </c>
       <c r="G509">
@@ -23265,10 +23265,10 @@
         <v>0</v>
       </c>
       <c r="I509">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J509">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K509">
         <v>0</v>
@@ -23290,17 +23290,17 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown San Juan River</t>
         </is>
       </c>
       <c r="E510" t="inlineStr">
         <is>
-          <t>Unknown Nitinat River</t>
+          <t>Unknown San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F510" t="inlineStr">
         <is>
-          <t>Unknown Nitinat River</t>
+          <t>Unknown San Juan River</t>
         </is>
       </c>
       <c r="G510">
@@ -23335,17 +23335,17 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E511" t="inlineStr">
         <is>
-          <t>Unknown San Juan River</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="F511" t="inlineStr">
         <is>
-          <t>Unknown San Juan River</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="G511">
@@ -23355,10 +23355,10 @@
         <v>0</v>
       </c>
       <c r="I511">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J511">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K511">
         <v>0</v>
@@ -23740,7 +23740,7 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>Hatchery NON-WCVI</t>
+          <t>Hatchery Unknown</t>
         </is>
       </c>
       <c r="E520" t="inlineStr">
@@ -24010,7 +24010,7 @@
       </c>
       <c r="D526" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E526" t="inlineStr">
@@ -24280,7 +24280,7 @@
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>Unknown NON-WCVI</t>
+          <t>Unknown Unknown</t>
         </is>
       </c>
       <c r="E532" t="inlineStr">
@@ -24370,12 +24370,12 @@
       </c>
       <c r="D534" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E534" t="inlineStr">
         <is>
-          <t>Natural Nitinat River</t>
+          <t>Natural Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F534" t="inlineStr">
@@ -24415,12 +24415,12 @@
       </c>
       <c r="D535" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E535" t="inlineStr">
         <is>
-          <t>Natural Robertson Creek</t>
+          <t>Natural Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F535" t="inlineStr">
@@ -24595,12 +24595,12 @@
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E539" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F539" t="inlineStr">
@@ -24775,12 +24775,12 @@
       </c>
       <c r="D543" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E543" t="inlineStr">
         <is>
-          <t>Hatchery Robertson Creek</t>
+          <t>Hatchery Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F543" t="inlineStr">
@@ -24820,7 +24820,7 @@
       </c>
       <c r="D544" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E544" t="inlineStr">
@@ -24865,12 +24865,12 @@
       </c>
       <c r="D545" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E545" t="inlineStr">
         <is>
-          <t>Unknown Nahmint River</t>
+          <t>Unknown Nahmint River (WCVI)</t>
         </is>
       </c>
       <c r="F545" t="inlineStr">
@@ -25000,12 +25000,12 @@
       </c>
       <c r="D548" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E548" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F548" t="inlineStr">
@@ -25360,12 +25360,12 @@
       </c>
       <c r="D556" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E556" t="inlineStr">
         <is>
-          <t>Natural Robertson Creek</t>
+          <t>Natural Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F556" t="inlineStr">
@@ -25630,7 +25630,7 @@
       </c>
       <c r="D562" t="inlineStr">
         <is>
-          <t>Natural NON-WCVI</t>
+          <t>Natural Unknown</t>
         </is>
       </c>
       <c r="E562" t="inlineStr">
@@ -25675,12 +25675,12 @@
       </c>
       <c r="D563" t="inlineStr">
         <is>
-          <t>Unknown WCVI</t>
+          <t>Unknown Other WCVI</t>
         </is>
       </c>
       <c r="E563" t="inlineStr">
         <is>
-          <t>Unknown Nitinat River</t>
+          <t>Unknown Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F563" t="inlineStr">
@@ -25810,12 +25810,12 @@
       </c>
       <c r="D566" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E566" t="inlineStr">
         <is>
-          <t>Hatchery Nitinat River</t>
+          <t>Hatchery Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F566" t="inlineStr">
@@ -25855,12 +25855,12 @@
       </c>
       <c r="D567" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E567" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F567" t="inlineStr">
@@ -26215,12 +26215,12 @@
       </c>
       <c r="D575" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E575" t="inlineStr">
         <is>
-          <t>Natural Robertson Creek</t>
+          <t>Natural Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F575" t="inlineStr">
@@ -26260,12 +26260,12 @@
       </c>
       <c r="D576" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural San Juan River</t>
         </is>
       </c>
       <c r="E576" t="inlineStr">
         <is>
-          <t>Natural San Juan River</t>
+          <t>Natural San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F576" t="inlineStr">
@@ -26530,12 +26530,12 @@
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E582" t="inlineStr">
         <is>
-          <t>Hatchery Sarita River</t>
+          <t>Hatchery Sarita River (WCVI)</t>
         </is>
       </c>
       <c r="F582" t="inlineStr">
@@ -26665,12 +26665,12 @@
       </c>
       <c r="D585" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E585" t="inlineStr">
         <is>
-          <t>Hatchery Conuma River</t>
+          <t>Hatchery Conuma River (WCVI)</t>
         </is>
       </c>
       <c r="F585" t="inlineStr">
@@ -26710,12 +26710,12 @@
       </c>
       <c r="D586" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E586" t="inlineStr">
         <is>
-          <t>Hatchery Sarita River</t>
+          <t>Hatchery Sarita River (WCVI)</t>
         </is>
       </c>
       <c r="F586" t="inlineStr">
@@ -26755,12 +26755,12 @@
       </c>
       <c r="D587" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery San Juan River</t>
         </is>
       </c>
       <c r="E587" t="inlineStr">
         <is>
-          <t>Hatchery San Juan River</t>
+          <t>Hatchery San Juan River (WCVI)</t>
         </is>
       </c>
       <c r="F587" t="inlineStr">
@@ -26890,12 +26890,12 @@
       </c>
       <c r="D590" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E590" t="inlineStr">
         <is>
-          <t>Hatchery Burman River</t>
+          <t>Hatchery Burman River (WCVI)</t>
         </is>
       </c>
       <c r="F590" t="inlineStr">
@@ -27115,12 +27115,12 @@
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E595" t="inlineStr">
         <is>
-          <t>Hatchery Conuma River</t>
+          <t>Hatchery Conuma River (WCVI)</t>
         </is>
       </c>
       <c r="F595" t="inlineStr">
@@ -27160,12 +27160,12 @@
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E596" t="inlineStr">
         <is>
-          <t>Natural Robertson Creek</t>
+          <t>Natural Robertson Creek (WCVI)</t>
         </is>
       </c>
       <c r="F596" t="inlineStr">
@@ -27295,12 +27295,12 @@
       </c>
       <c r="D599" t="inlineStr">
         <is>
-          <t>Hatchery WCVI</t>
+          <t>Hatchery Other WCVI</t>
         </is>
       </c>
       <c r="E599" t="inlineStr">
         <is>
-          <t>Hatchery Conuma River</t>
+          <t>Hatchery Conuma River (WCVI)</t>
         </is>
       </c>
       <c r="F599" t="inlineStr">
@@ -27745,12 +27745,12 @@
       </c>
       <c r="D609" t="inlineStr">
         <is>
-          <t>Natural WCVI</t>
+          <t>Natural Other WCVI</t>
         </is>
       </c>
       <c r="E609" t="inlineStr">
         <is>
-          <t>Natural Nitinat River</t>
+          <t>Natural Nitinat River (WCVI)</t>
         </is>
       </c>
       <c r="F609" t="inlineStr">

</xml_diff>